<commit_message>
Results after investigating 528 ok pairs
</commit_message>
<xml_diff>
--- a/results/common_good_pairs_fixed_nicadfse13_2016-07-17.xlsx
+++ b/results/common_good_pairs_fixed_nicadfse13_2016-07-17.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="13500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26980" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="16" r:id="rId1"/>
@@ -553,7 +553,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6:P7"/>
+      <selection activeCell="P1" sqref="P1:Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,52 +577,52 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2">
-        <v>0.94117647058823495</v>
+        <v>0.9</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="D1">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="E1">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="G1">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H1">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="J1">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="K1">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="M1">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="N1">
+        <v>33</v>
+      </c>
+      <c r="P1" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="8" t="s">
-        <v>45</v>
-      </c>
       <c r="Q1" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -630,49 +630,49 @@
         <v>35</v>
       </c>
       <c r="B2" s="2">
-        <v>0.94117647058823495</v>
+        <v>0.90909090909090895</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D2">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E2">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="G2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H2">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="J2">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="K2">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="M2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="N2">
-        <v>51</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+      <c r="P2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -680,199 +680,199 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>0.90909090909090895</v>
+        <v>0.8125</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G3">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H3">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="J3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K3">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="M3">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="N3">
-        <v>53</v>
-      </c>
-      <c r="P3" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>56</v>
+        <v>61</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2">
-        <v>0.8125</v>
+        <v>0.71428571428571397</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
       <c r="G4">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H4">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="J4">
         <v>12</v>
       </c>
       <c r="K4">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="L4" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="M4">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N4">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2">
-        <v>0.8125</v>
+        <v>0.71428571428571397</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D5">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="E5">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="G5">
-        <v>49</v>
+        <v>76</v>
       </c>
       <c r="H5">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="J5">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="K5">
+        <v>17</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5">
+        <v>75</v>
+      </c>
+      <c r="N5">
+        <v>81</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="L5" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5">
-        <v>49</v>
-      </c>
-      <c r="N5">
-        <v>61</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2">
-        <v>0.76470588235294101</v>
+        <v>0.71428571428571397</v>
       </c>
       <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
         <v>13</v>
       </c>
-      <c r="D6">
+      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6">
+        <v>107</v>
+      </c>
+      <c r="H6">
+        <v>113</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6">
+        <v>106</v>
+      </c>
+      <c r="N6">
+        <v>112</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="E6">
-        <v>66</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6">
-        <v>47</v>
-      </c>
-      <c r="H6">
-        <v>63</v>
-      </c>
-      <c r="I6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6">
-        <v>51</v>
-      </c>
-      <c r="K6">
-        <v>63</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6">
-        <v>48</v>
-      </c>
-      <c r="N6">
-        <v>60</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -880,49 +880,49 @@
         <v>35</v>
       </c>
       <c r="B7" s="2">
-        <v>0.76470588235294101</v>
+        <v>0.94117647058823495</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="E7">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G7">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <v>52</v>
+      </c>
+      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>17</v>
+      </c>
+      <c r="K7">
+        <v>32</v>
+      </c>
+      <c r="L7" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>36</v>
+      </c>
+      <c r="N7">
         <v>51</v>
       </c>
-      <c r="H7">
-        <v>67</v>
-      </c>
-      <c r="I7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7">
-        <v>51</v>
-      </c>
-      <c r="K7">
-        <v>63</v>
-      </c>
-      <c r="L7" t="s">
-        <v>16</v>
-      </c>
-      <c r="M7">
-        <v>52</v>
-      </c>
-      <c r="N7">
-        <v>64</v>
-      </c>
-      <c r="P7" s="7" t="s">
+      <c r="P7" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="Q7" s="7" t="s">
-        <v>46</v>
+      <c r="Q7" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -980,49 +980,49 @@
         <v>35</v>
       </c>
       <c r="B9" s="2">
-        <v>0.7</v>
+        <v>0.8125</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D9">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="E9">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G9">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="H9">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J9">
-        <v>98</v>
+        <v>38</v>
       </c>
       <c r="K9">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="L9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="M9">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="N9">
-        <v>75</v>
-      </c>
-      <c r="P9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q9" s="7" t="s">
-        <v>49</v>
+        <v>61</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -1030,249 +1030,249 @@
         <v>36</v>
       </c>
       <c r="B10" s="2">
-        <v>0.71428571428571397</v>
+        <v>0.85714285714285698</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D10">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="E10">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="G10">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="H10">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="J10">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="K10">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="L10" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="M10">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="N10">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.94117647058823495</v>
+      </c>
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>45</v>
+      </c>
+      <c r="E11">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11">
         <v>36</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.71428571428571397</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11">
-        <v>13</v>
-      </c>
-      <c r="E11">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11">
-        <v>107</v>
-      </c>
       <c r="H11">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="J11">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="K11">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="L11" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <v>106</v>
+        <v>36</v>
       </c>
       <c r="N11">
-        <v>112</v>
+        <v>51</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>45</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="2">
-        <v>0.71428571428571397</v>
+        <v>0.76470588235294101</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D12">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E12">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="G12">
+        <v>47</v>
+      </c>
+      <c r="H12">
+        <v>63</v>
+      </c>
+      <c r="I12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12">
         <v>51</v>
       </c>
-      <c r="H12">
-        <v>57</v>
-      </c>
-      <c r="I12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12">
-        <v>12</v>
-      </c>
       <c r="K12">
-        <v>17</v>
+        <v>63</v>
       </c>
       <c r="L12" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="M12">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="N12">
-        <v>56</v>
-      </c>
-      <c r="P12" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="Q12" s="8" t="s">
-        <v>50</v>
+      <c r="Q12" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="2">
-        <v>0.85714285714285698</v>
+        <v>0.76470588235294101</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="D13">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E13">
+        <v>66</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13">
+        <v>51</v>
+      </c>
+      <c r="H13">
+        <v>67</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13">
+        <v>51</v>
+      </c>
+      <c r="K13">
+        <v>63</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13">
+        <v>52</v>
+      </c>
+      <c r="N13">
+        <v>64</v>
+      </c>
+      <c r="P13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13">
-        <v>85</v>
-      </c>
-      <c r="H13">
-        <v>91</v>
-      </c>
-      <c r="I13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13">
-        <v>39</v>
-      </c>
-      <c r="K13">
-        <v>44</v>
-      </c>
-      <c r="L13" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13">
-        <v>85</v>
-      </c>
-      <c r="N13">
-        <v>90</v>
-      </c>
-      <c r="P13" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q13" s="8" t="s">
-        <v>52</v>
+      <c r="Q13" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="E14">
+        <v>104</v>
+      </c>
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>66</v>
+      </c>
+      <c r="H14">
+        <v>74</v>
+      </c>
+      <c r="I14" t="s">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14">
-        <v>25</v>
-      </c>
-      <c r="H14">
-        <v>34</v>
-      </c>
-      <c r="I14" t="s">
-        <v>33</v>
-      </c>
       <c r="J14">
-        <v>3</v>
+        <v>98</v>
       </c>
       <c r="K14">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="L14" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="M14">
-        <v>25</v>
+        <v>68</v>
       </c>
       <c r="N14">
-        <v>33</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q14" s="8" t="s">
-        <v>53</v>
+        <v>75</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -1346,14 +1346,15 @@
       <c r="F22" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A1:P22">
-    <sortCondition ref="O1:O22"/>
-    <sortCondition ref="F1:F22"/>
-    <sortCondition ref="G1:G22"/>
-    <sortCondition ref="H1:H22"/>
-    <sortCondition ref="C1:C22"/>
-    <sortCondition ref="D1:D22"/>
-    <sortCondition ref="E1:E22"/>
+  <sortState ref="A1:Q14">
+    <sortCondition ref="D1:D14"/>
+    <sortCondition ref="E1:E14"/>
+    <sortCondition ref="G1:G14"/>
+    <sortCondition ref="H1:H14"/>
+    <sortCondition ref="J1:J14"/>
+    <sortCondition ref="K1:K14"/>
+    <sortCondition ref="M1:M14"/>
+    <sortCondition ref="N1:N14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated after finishing analysing 528 ok pairs (fixed some problems)
</commit_message>
<xml_diff>
--- a/results/common_good_pairs_fixed_nicadfse13_2016-07-17.xlsx
+++ b/results/common_good_pairs_fixed_nicadfse13_2016-07-17.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="16" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="60">
   <si>
     <t>stackoverflow_formatted/11187462_0.java</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Both fragments are copied from http://www.rgagnon.com/javadetails/java-0426.html</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -552,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P1" sqref="P1:Q14"/>
     </sheetView>
   </sheetViews>
@@ -1362,10 +1365,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD24"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1374,18 +1377,18 @@
     <col min="2" max="2" width="36.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="86.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.83203125" customWidth="1"/>
     <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
         <v>0.94117647058823495</v>
       </c>
@@ -1425,8 +1428,11 @@
       <c r="M1">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0.94117647058823495</v>
       </c>
@@ -1466,8 +1472,11 @@
       <c r="M2">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0.90909090909090895</v>
       </c>
@@ -1507,8 +1516,11 @@
       <c r="M3">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0.8125</v>
       </c>
@@ -1548,8 +1560,11 @@
       <c r="M4">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0.8125</v>
       </c>
@@ -1589,8 +1604,11 @@
       <c r="M5">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0.76470588235294101</v>
       </c>
@@ -1630,8 +1648,11 @@
       <c r="M6">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0.76470588235294101</v>
       </c>
@@ -1671,8 +1692,11 @@
       <c r="M7">
         <v>64</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0.76470588235294101</v>
       </c>
@@ -1712,8 +1736,11 @@
       <c r="M8">
         <v>131</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>0.7</v>
       </c>
@@ -1753,8 +1780,11 @@
       <c r="M9">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>0.90909090909090895</v>
       </c>
@@ -1794,8 +1824,11 @@
       <c r="M11" s="5">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N11" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>0.76470588235294101</v>
       </c>
@@ -1835,8 +1868,11 @@
       <c r="M12" s="5">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N12" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>0.76470588235294101</v>
       </c>
@@ -1876,13 +1912,16 @@
       <c r="M13" s="5">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>0.94117647058823495</v>
       </c>
@@ -2261,10 +2300,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD15"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2273,18 +2312,16 @@
     <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.6640625" customWidth="1"/>
+    <col min="6" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="86.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.33203125" customWidth="1"/>
+    <col min="12" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
         <v>0.94117647058823495</v>
       </c>
@@ -2325,7 +2362,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0.94117647058823495</v>
       </c>
@@ -2366,7 +2403,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0.90909090909090895</v>
       </c>
@@ -2407,7 +2444,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0.8125</v>
       </c>
@@ -2448,7 +2485,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0.8125</v>
       </c>
@@ -2489,7 +2526,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0.76470588235294101</v>
       </c>
@@ -2530,7 +2567,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0.76470588235294101</v>
       </c>
@@ -2571,7 +2608,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0.76470588235294101</v>
       </c>
@@ -2612,7 +2649,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>0.7</v>
       </c>
@@ -2653,7 +2690,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>0.71428571428571397</v>
       </c>
@@ -2693,8 +2730,11 @@
       <c r="M11">
         <v>81</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>0.71428571428571397</v>
       </c>
@@ -2734,8 +2774,11 @@
       <c r="M12">
         <v>112</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>0.71428571428571397</v>
       </c>
@@ -2775,8 +2818,11 @@
       <c r="M13">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>0.85714285714285698</v>
       </c>
@@ -2816,8 +2862,11 @@
       <c r="M14">
         <v>90</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>0.9</v>
       </c>
@@ -2856,6 +2905,9 @@
       </c>
       <c r="M15">
         <v>33</v>
+      </c>
+      <c r="N15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -2873,10 +2925,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2885,18 +2937,18 @@
     <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" customWidth="1"/>
     <col min="6" max="6" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="86.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="41.33203125" customWidth="1"/>
     <col min="12" max="12" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
         <v>0.94117647058823495</v>
       </c>
@@ -2937,7 +2989,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>0.94117647058823495</v>
       </c>
@@ -2978,7 +3030,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0.90909090909090895</v>
       </c>
@@ -3019,7 +3071,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0.8125</v>
       </c>
@@ -3060,7 +3112,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0.8125</v>
       </c>
@@ -3101,7 +3153,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0.76470588235294101</v>
       </c>
@@ -3142,7 +3194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0.76470588235294101</v>
       </c>
@@ -3183,7 +3235,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0.76470588235294101</v>
       </c>
@@ -3224,7 +3276,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>0.7</v>
       </c>
@@ -3265,7 +3317,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>0.9</v>
       </c>
@@ -3305,8 +3357,11 @@
       <c r="M11">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -3318,10 +3373,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3330,16 +3385,16 @@
     <col min="2" max="2" width="36.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="104.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" customWidth="1"/>
     <col min="6" max="7" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="36.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="104.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.5" customWidth="1"/>
+    <col min="12" max="13" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6">
         <v>0.90909090909090895</v>
       </c>
@@ -3379,8 +3434,11 @@
       <c r="M1" s="3">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>0.76470588235294101</v>
       </c>
@@ -3420,8 +3478,11 @@
       <c r="M2" s="3">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="N2" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>0.76470588235294101</v>
       </c>
@@ -3461,8 +3522,11 @@
       <c r="M3" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>0.71428571428571397</v>
       </c>
@@ -3503,7 +3567,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0.71428571428571397</v>
       </c>
@@ -3544,7 +3608,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>0.71428571428571397</v>
       </c>
@@ -3585,7 +3649,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>0.85714285714285698</v>
       </c>
@@ -3626,7 +3690,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>0.9</v>
       </c>
@@ -3667,7 +3731,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>23</v>
       </c>

</xml_diff>